<commit_message>
lots of work on closures
</commit_message>
<xml_diff>
--- a/data/washington/da_sampling/tables/TableSX_sample_size.xlsx
+++ b/data/washington/da_sampling/tables/TableSX_sample_size.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/domoic_acid_mgmt/data/washington/da_sampling/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED211416-DB44-0946-A59A-EF5565D92C29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD72F4FB-B0C9-1F4D-97A9-EAAAFBBE5229}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20980" yWindow="10080" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5040" yWindow="6080" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableSX_sample_size" sheetId="1" r:id="rId1"/>
@@ -594,13 +594,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -959,7 +959,7 @@
   <dimension ref="A2:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E17"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -971,12 +971,12 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -999,16 +999,16 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>12963</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>5197</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>3883</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>3883</v>
       </c>
     </row>
@@ -1016,16 +1016,16 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>7445</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>2425</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>2510</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>2510</v>
       </c>
     </row>
@@ -1033,16 +1033,16 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>3180</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>62</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>1559</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>1559</v>
       </c>
     </row>
@@ -1050,16 +1050,16 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>1731</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>1731</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1067,16 +1067,16 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>1055</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>343</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>356</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>356</v>
       </c>
     </row>
@@ -1084,16 +1084,16 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>234</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>18</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>108</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>108</v>
       </c>
     </row>
@@ -1101,16 +1101,16 @@
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>32</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>10</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>11</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>11</v>
       </c>
     </row>
@@ -1118,16 +1118,16 @@
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>22</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>6</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>8</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>8</v>
       </c>
     </row>
@@ -1135,16 +1135,16 @@
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>9</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>3</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>3</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>3</v>
       </c>
     </row>
@@ -1152,16 +1152,16 @@
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>7</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>3</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>3</v>
       </c>
     </row>
@@ -1169,16 +1169,16 @@
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>4</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>4</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>0</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1186,53 +1186,53 @@
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>2</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>0</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>1</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>2</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>0</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>1</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <f>SUM(B4:B16)</f>
         <v>26686</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <f t="shared" ref="C17:E17" si="0">SUM(C4:C16)</f>
         <v>9800</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <f t="shared" si="0"/>
         <v>8443</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <f t="shared" si="0"/>
         <v>8443</v>
       </c>

</xml_diff>